<commit_message>
near to be completed. waiting for definite input file and signal condition
</commit_message>
<xml_diff>
--- a/Data/Alert RATING Stoxx600 20191203.xlsx
+++ b/Data/Alert RATING Stoxx600 20191203.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="91">
   <si>
     <t>FactSet Universal Screening</t>
   </si>
@@ -274,6 +274,24 @@
   </si>
   <si>
     <t>Bernstein_RATING</t>
+  </si>
+  <si>
+    <t>ISIN</t>
+  </si>
+  <si>
+    <t>GB0002162385</t>
+  </si>
+  <si>
+    <t>GB0001367019</t>
+  </si>
+  <si>
+    <t>GB0002652740</t>
+  </si>
+  <si>
+    <t>GB00BF5H9P87</t>
+  </si>
+  <si>
+    <t>GB00BYW0PQ60</t>
   </si>
 </sst>
 </file>
@@ -684,39 +702,39 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BV11"/>
+  <dimension ref="A1:BW11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5:XFD5"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="74" width="14.28515625" customWidth="1"/>
+    <col min="2" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="75" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:74" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:75" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:74" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:75" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:74" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:75" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:74" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:75" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:74" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:75" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -724,287 +742,290 @@
         <v>13</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="H5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="I5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="J5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="K5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="L5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="M5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="M5" s="6" t="s">
+      <c r="N5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="O5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="O5" s="6" t="s">
+      <c r="P5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="P5" s="6" t="s">
+      <c r="Q5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="Q5" s="6" t="s">
+      <c r="R5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="R5" s="6" t="s">
+      <c r="S5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="S5" s="6" t="s">
+      <c r="T5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="T5" s="6" t="s">
+      <c r="U5" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="U5" s="6" t="s">
+      <c r="V5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="V5" s="6" t="s">
+      <c r="W5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="W5" s="6" t="s">
+      <c r="X5" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="X5" s="6" t="s">
+      <c r="Y5" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="Y5" s="6" t="s">
+      <c r="Z5" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="Z5" s="6" t="s">
+      <c r="AA5" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="AA5" s="6" t="s">
+      <c r="AB5" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="AB5" s="6" t="s">
+      <c r="AC5" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="AC5" s="6" t="s">
+      <c r="AD5" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="AD5" s="6" t="s">
+      <c r="AE5" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="AE5" s="6" t="s">
+      <c r="AF5" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="AF5" s="6" t="s">
+      <c r="AG5" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="AG5" s="6" t="s">
+      <c r="AH5" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="AH5" s="6" t="s">
+      <c r="AI5" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="AI5" s="6" t="s">
+      <c r="AJ5" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="AJ5" s="6" t="s">
+      <c r="AK5" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AK5" s="6" t="s">
+      <c r="AL5" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="AL5" s="6" t="s">
+      <c r="AM5" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="AM5" s="6" t="s">
+      <c r="AN5" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="AN5" s="6" t="s">
+      <c r="AO5" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="AO5" s="6" t="s">
+      <c r="AP5" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="AP5" s="6" t="s">
+      <c r="AQ5" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="AQ5" s="6" t="s">
+      <c r="AR5" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AR5" s="6" t="s">
+      <c r="AS5" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="AS5" s="6" t="s">
+      <c r="AT5" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="AT5" s="6" t="s">
+      <c r="AU5" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="AU5" s="6" t="s">
+      <c r="AV5" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="AV5" s="6" t="s">
+      <c r="AW5" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="AW5" s="6" t="s">
+      <c r="AX5" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="AX5" s="6" t="s">
+      <c r="AY5" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="AY5" s="6" t="s">
+      <c r="AZ5" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="AZ5" s="6" t="s">
+      <c r="BA5" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="BA5" s="6" t="s">
+      <c r="BB5" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="BB5" s="6" t="s">
+      <c r="BC5" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="BC5" s="6" t="s">
+      <c r="BD5" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="BD5" s="6" t="s">
+      <c r="BE5" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="BE5" s="6" t="s">
+      <c r="BF5" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="BF5" s="6" t="s">
+      <c r="BG5" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="BG5" s="6" t="s">
+      <c r="BH5" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="BH5" s="6" t="s">
+      <c r="BI5" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="BI5" s="6" t="s">
+      <c r="BJ5" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="BJ5" s="6" t="s">
+      <c r="BK5" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="BK5" s="6" t="s">
+      <c r="BL5" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="BL5" s="6" t="s">
+      <c r="BM5" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="BM5" s="6" t="s">
+      <c r="BN5" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="BN5" s="6" t="s">
+      <c r="BO5" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="BO5" s="6" t="s">
+      <c r="BP5" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="BP5" s="6" t="s">
+      <c r="BQ5" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="BQ5" s="6" t="s">
+      <c r="BR5" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="BR5" s="6" t="s">
+      <c r="BS5" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="BS5" s="6" t="s">
+      <c r="BT5" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="BT5" s="6" t="s">
+      <c r="BU5" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="BU5" s="6" t="s">
+      <c r="BV5" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="BV5" s="6"/>
+      <c r="BW5" s="6"/>
     </row>
-    <row r="6" spans="1:74" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:75" ht="12.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="4"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="3"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="3"/>
       <c r="I6" s="4"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="3"/>
       <c r="L6" s="4"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="3"/>
       <c r="O6" s="4"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="3"/>
       <c r="R6" s="4"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="3"/>
       <c r="U6" s="4"/>
-      <c r="V6" s="3"/>
-      <c r="W6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="3"/>
       <c r="X6" s="4"/>
-      <c r="Y6" s="3"/>
-      <c r="Z6" s="4"/>
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="3"/>
       <c r="AA6" s="4"/>
-      <c r="AB6" s="3"/>
-      <c r="AC6" s="4"/>
+      <c r="AB6" s="4"/>
+      <c r="AC6" s="3"/>
       <c r="AD6" s="4"/>
-      <c r="AE6" s="3"/>
-      <c r="AF6" s="4"/>
+      <c r="AE6" s="4"/>
+      <c r="AF6" s="3"/>
       <c r="AG6" s="4"/>
-      <c r="AH6" s="3"/>
-      <c r="AI6" s="4"/>
+      <c r="AH6" s="4"/>
+      <c r="AI6" s="3"/>
       <c r="AJ6" s="4"/>
-      <c r="AK6" s="3"/>
-      <c r="AL6" s="4"/>
+      <c r="AK6" s="4"/>
+      <c r="AL6" s="3"/>
       <c r="AM6" s="4"/>
-      <c r="AN6" s="3"/>
-      <c r="AO6" s="4"/>
+      <c r="AN6" s="4"/>
+      <c r="AO6" s="3"/>
       <c r="AP6" s="4"/>
-      <c r="AQ6" s="3"/>
-      <c r="AR6" s="4"/>
+      <c r="AQ6" s="4"/>
+      <c r="AR6" s="3"/>
       <c r="AS6" s="4"/>
-      <c r="AT6" s="3"/>
-      <c r="AU6" s="4"/>
+      <c r="AT6" s="4"/>
+      <c r="AU6" s="3"/>
       <c r="AV6" s="4"/>
-      <c r="AW6" s="3"/>
-      <c r="AX6" s="4"/>
+      <c r="AW6" s="4"/>
+      <c r="AX6" s="3"/>
       <c r="AY6" s="4"/>
-      <c r="AZ6" s="3"/>
-      <c r="BA6" s="4"/>
+      <c r="AZ6" s="4"/>
+      <c r="BA6" s="3"/>
       <c r="BB6" s="4"/>
-      <c r="BC6" s="3"/>
-      <c r="BD6" s="4"/>
+      <c r="BC6" s="4"/>
+      <c r="BD6" s="3"/>
       <c r="BE6" s="4"/>
-      <c r="BF6" s="3"/>
-      <c r="BG6" s="4"/>
+      <c r="BF6" s="4"/>
+      <c r="BG6" s="3"/>
       <c r="BH6" s="4"/>
-      <c r="BI6" s="3"/>
-      <c r="BJ6" s="4"/>
+      <c r="BI6" s="4"/>
+      <c r="BJ6" s="3"/>
       <c r="BK6" s="4"/>
-      <c r="BL6" s="3"/>
-      <c r="BM6" s="4"/>
-      <c r="BN6" s="3"/>
+      <c r="BL6" s="4"/>
+      <c r="BM6" s="3"/>
+      <c r="BN6" s="4"/>
       <c r="BO6" s="3"/>
       <c r="BP6" s="3"/>
       <c r="BQ6" s="3"/>
@@ -1013,8 +1034,9 @@
       <c r="BT6" s="3"/>
       <c r="BU6" s="3"/>
       <c r="BV6" s="3"/>
+      <c r="BW6" s="3"/>
     </row>
-    <row r="7" spans="1:74" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:75" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -1022,195 +1044,195 @@
         <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="3">
+      <c r="E7" s="3">
         <v>7.3965490000000003</v>
       </c>
-      <c r="E7" s="4">
+      <c r="F7" s="4">
         <v>1</v>
       </c>
-      <c r="F7" s="4">
-        <v>0</v>
-      </c>
-      <c r="G7" s="3">
+      <c r="G7" s="4">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3">
         <v>1</v>
       </c>
-      <c r="H7" s="4">
-        <v>0</v>
-      </c>
       <c r="I7" s="4">
         <v>0</v>
       </c>
-      <c r="J7" s="3">
-        <v>0</v>
-      </c>
-      <c r="K7" s="4">
+      <c r="J7" s="4">
+        <v>0</v>
+      </c>
+      <c r="K7" s="3">
         <v>0</v>
       </c>
       <c r="L7" s="4">
         <v>0</v>
       </c>
-      <c r="M7" s="3">
-        <v>0</v>
-      </c>
-      <c r="N7" s="4">
+      <c r="M7" s="4">
+        <v>0</v>
+      </c>
+      <c r="N7" s="3">
         <v>0</v>
       </c>
       <c r="O7" s="4">
         <v>0</v>
       </c>
-      <c r="P7" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="4">
+      <c r="P7" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="3">
         <v>0</v>
       </c>
       <c r="R7" s="4">
         <v>0</v>
       </c>
-      <c r="S7" s="3">
-        <v>0</v>
-      </c>
-      <c r="T7" s="4">
+      <c r="S7" s="4">
+        <v>0</v>
+      </c>
+      <c r="T7" s="3">
         <v>0</v>
       </c>
       <c r="U7" s="4">
         <v>0</v>
       </c>
-      <c r="V7" s="3">
-        <v>0</v>
-      </c>
-      <c r="W7" s="4">
+      <c r="V7" s="4">
+        <v>0</v>
+      </c>
+      <c r="W7" s="3">
         <v>0</v>
       </c>
       <c r="X7" s="4">
         <v>0</v>
       </c>
-      <c r="Y7" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="4">
+      <c r="Y7" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="3">
         <v>0</v>
       </c>
       <c r="AA7" s="4">
         <v>0</v>
       </c>
-      <c r="AB7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC7" s="4">
+      <c r="AB7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="3">
         <v>0</v>
       </c>
       <c r="AD7" s="4">
         <v>0</v>
       </c>
-      <c r="AE7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF7" s="4">
+      <c r="AE7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="3">
         <v>0</v>
       </c>
       <c r="AG7" s="4">
         <v>0</v>
       </c>
-      <c r="AH7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AI7" s="4">
+      <c r="AH7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="3">
         <v>0</v>
       </c>
       <c r="AJ7" s="4">
         <v>0</v>
       </c>
-      <c r="AK7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AL7" s="4">
+      <c r="AK7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL7" s="3">
         <v>0</v>
       </c>
       <c r="AM7" s="4">
         <v>0</v>
       </c>
-      <c r="AN7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AO7" s="4">
+      <c r="AN7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AO7" s="3">
         <v>0</v>
       </c>
       <c r="AP7" s="4">
         <v>0</v>
       </c>
-      <c r="AQ7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AR7" s="4">
+      <c r="AQ7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR7" s="3">
         <v>0</v>
       </c>
       <c r="AS7" s="4">
         <v>0</v>
       </c>
-      <c r="AT7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AU7" s="4">
+      <c r="AT7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AU7" s="3">
         <v>0</v>
       </c>
       <c r="AV7" s="4">
         <v>0</v>
       </c>
-      <c r="AW7" s="3">
-        <v>0</v>
-      </c>
-      <c r="AX7" s="4">
+      <c r="AW7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AX7" s="3">
         <v>0</v>
       </c>
       <c r="AY7" s="4">
         <v>0</v>
       </c>
-      <c r="AZ7" s="3">
-        <v>0</v>
-      </c>
-      <c r="BA7" s="4">
+      <c r="AZ7" s="4">
+        <v>0</v>
+      </c>
+      <c r="BA7" s="3">
         <v>0</v>
       </c>
       <c r="BB7" s="4">
         <v>0</v>
       </c>
-      <c r="BC7" s="3">
-        <v>0</v>
-      </c>
-      <c r="BD7" s="4">
+      <c r="BC7" s="4">
+        <v>0</v>
+      </c>
+      <c r="BD7" s="3">
         <v>0</v>
       </c>
       <c r="BE7" s="4">
         <v>0</v>
       </c>
-      <c r="BF7" s="3">
-        <v>0</v>
-      </c>
-      <c r="BG7" s="4">
+      <c r="BF7" s="4">
+        <v>0</v>
+      </c>
+      <c r="BG7" s="3">
         <v>0</v>
       </c>
       <c r="BH7" s="4">
         <v>0</v>
       </c>
-      <c r="BI7" s="3">
-        <v>0</v>
-      </c>
-      <c r="BJ7" s="4">
+      <c r="BI7" s="4">
+        <v>0</v>
+      </c>
+      <c r="BJ7" s="3">
         <v>0</v>
       </c>
       <c r="BK7" s="4">
         <v>0</v>
       </c>
-      <c r="BL7" s="3">
-        <v>0</v>
-      </c>
-      <c r="BM7" s="4">
-        <v>0</v>
-      </c>
-      <c r="BN7" s="3">
+      <c r="BL7" s="4">
+        <v>0</v>
+      </c>
+      <c r="BM7" s="3">
+        <v>0</v>
+      </c>
+      <c r="BN7" s="4">
         <v>0</v>
       </c>
       <c r="BO7" s="3">
@@ -1235,10 +1257,13 @@
         <v>0</v>
       </c>
       <c r="BV7" s="3">
+        <v>0</v>
+      </c>
+      <c r="BW7" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:74" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:75" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -1246,195 +1271,195 @@
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="3">
+      <c r="E8" s="3">
         <v>5.181705</v>
-      </c>
-      <c r="E8" s="4">
-        <v>-1</v>
       </c>
       <c r="F8" s="4">
         <v>-1</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="4">
         <v>-1</v>
       </c>
-      <c r="H8" s="4">
-        <v>0</v>
+      <c r="H8" s="3">
+        <v>-1</v>
       </c>
       <c r="I8" s="4">
         <v>0</v>
       </c>
-      <c r="J8" s="3">
-        <v>0</v>
-      </c>
-      <c r="K8" s="4">
+      <c r="J8" s="4">
+        <v>0</v>
+      </c>
+      <c r="K8" s="3">
         <v>0</v>
       </c>
       <c r="L8" s="4">
         <v>0</v>
       </c>
-      <c r="M8" s="3">
-        <v>0</v>
-      </c>
-      <c r="N8" s="4">
+      <c r="M8" s="4">
+        <v>0</v>
+      </c>
+      <c r="N8" s="3">
         <v>0</v>
       </c>
       <c r="O8" s="4">
         <v>0</v>
       </c>
-      <c r="P8" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="4">
+      <c r="P8" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="3">
         <v>0</v>
       </c>
       <c r="R8" s="4">
         <v>0</v>
       </c>
-      <c r="S8" s="3">
-        <v>0</v>
-      </c>
-      <c r="T8" s="4">
+      <c r="S8" s="4">
+        <v>0</v>
+      </c>
+      <c r="T8" s="3">
         <v>0</v>
       </c>
       <c r="U8" s="4">
         <v>0</v>
       </c>
-      <c r="V8" s="3">
-        <v>0</v>
-      </c>
-      <c r="W8" s="4">
+      <c r="V8" s="4">
+        <v>0</v>
+      </c>
+      <c r="W8" s="3">
         <v>0</v>
       </c>
       <c r="X8" s="4">
         <v>0</v>
       </c>
-      <c r="Y8" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="4">
+      <c r="Y8" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="3">
         <v>0</v>
       </c>
       <c r="AA8" s="4">
         <v>0</v>
       </c>
-      <c r="AB8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC8" s="4">
+      <c r="AB8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="3">
         <v>0</v>
       </c>
       <c r="AD8" s="4">
         <v>0</v>
       </c>
-      <c r="AE8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF8" s="4">
+      <c r="AE8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="3">
         <v>0</v>
       </c>
       <c r="AG8" s="4">
         <v>0</v>
       </c>
-      <c r="AH8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AI8" s="4">
+      <c r="AH8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI8" s="3">
         <v>0</v>
       </c>
       <c r="AJ8" s="4">
         <v>0</v>
       </c>
-      <c r="AK8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AL8" s="4">
+      <c r="AK8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL8" s="3">
         <v>0</v>
       </c>
       <c r="AM8" s="4">
         <v>0</v>
       </c>
-      <c r="AN8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AO8" s="4">
+      <c r="AN8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AO8" s="3">
         <v>0</v>
       </c>
       <c r="AP8" s="4">
         <v>0</v>
       </c>
-      <c r="AQ8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AR8" s="4">
+      <c r="AQ8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR8" s="3">
         <v>0</v>
       </c>
       <c r="AS8" s="4">
         <v>0</v>
       </c>
-      <c r="AT8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AU8" s="4">
+      <c r="AT8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AU8" s="3">
         <v>0</v>
       </c>
       <c r="AV8" s="4">
         <v>0</v>
       </c>
-      <c r="AW8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AX8" s="4">
+      <c r="AW8" s="4">
+        <v>0</v>
+      </c>
+      <c r="AX8" s="3">
         <v>0</v>
       </c>
       <c r="AY8" s="4">
         <v>0</v>
       </c>
-      <c r="AZ8" s="3">
-        <v>0</v>
-      </c>
-      <c r="BA8" s="4">
+      <c r="AZ8" s="4">
+        <v>0</v>
+      </c>
+      <c r="BA8" s="3">
         <v>0</v>
       </c>
       <c r="BB8" s="4">
         <v>0</v>
       </c>
-      <c r="BC8" s="3">
-        <v>0</v>
-      </c>
-      <c r="BD8" s="4">
+      <c r="BC8" s="4">
+        <v>0</v>
+      </c>
+      <c r="BD8" s="3">
         <v>0</v>
       </c>
       <c r="BE8" s="4">
         <v>0</v>
       </c>
-      <c r="BF8" s="3">
-        <v>0</v>
-      </c>
-      <c r="BG8" s="4">
+      <c r="BF8" s="4">
+        <v>0</v>
+      </c>
+      <c r="BG8" s="3">
         <v>0</v>
       </c>
       <c r="BH8" s="4">
         <v>0</v>
       </c>
-      <c r="BI8" s="3">
-        <v>0</v>
-      </c>
-      <c r="BJ8" s="4">
+      <c r="BI8" s="4">
+        <v>0</v>
+      </c>
+      <c r="BJ8" s="3">
         <v>0</v>
       </c>
       <c r="BK8" s="4">
         <v>0</v>
       </c>
-      <c r="BL8" s="3">
-        <v>0</v>
-      </c>
-      <c r="BM8" s="4">
-        <v>0</v>
-      </c>
-      <c r="BN8" s="3">
+      <c r="BL8" s="4">
+        <v>0</v>
+      </c>
+      <c r="BM8" s="3">
+        <v>0</v>
+      </c>
+      <c r="BN8" s="4">
         <v>0</v>
       </c>
       <c r="BO8" s="3">
@@ -1459,10 +1484,13 @@
         <v>0</v>
       </c>
       <c r="BV8" s="3">
+        <v>0</v>
+      </c>
+      <c r="BW8" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:74" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:75" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -1470,195 +1498,195 @@
         <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="3">
+      <c r="E9" s="3">
         <v>47.438870000000001</v>
       </c>
-      <c r="E9" s="4">
+      <c r="F9" s="4">
         <v>1</v>
       </c>
-      <c r="F9" s="4">
-        <v>0</v>
-      </c>
-      <c r="G9" s="3">
+      <c r="G9" s="4">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3">
         <v>1</v>
       </c>
-      <c r="H9" s="4">
-        <v>0</v>
-      </c>
       <c r="I9" s="4">
         <v>0</v>
       </c>
-      <c r="J9" s="3">
-        <v>0</v>
-      </c>
-      <c r="K9" s="4">
+      <c r="J9" s="4">
+        <v>0</v>
+      </c>
+      <c r="K9" s="3">
         <v>0</v>
       </c>
       <c r="L9" s="4">
         <v>0</v>
       </c>
-      <c r="M9" s="3">
-        <v>0</v>
-      </c>
-      <c r="N9" s="4">
+      <c r="M9" s="4">
+        <v>0</v>
+      </c>
+      <c r="N9" s="3">
         <v>0</v>
       </c>
       <c r="O9" s="4">
         <v>0</v>
       </c>
-      <c r="P9" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="4">
+      <c r="P9" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="3">
         <v>0</v>
       </c>
       <c r="R9" s="4">
         <v>0</v>
       </c>
-      <c r="S9" s="3">
-        <v>0</v>
-      </c>
-      <c r="T9" s="4">
+      <c r="S9" s="4">
+        <v>0</v>
+      </c>
+      <c r="T9" s="3">
         <v>0</v>
       </c>
       <c r="U9" s="4">
         <v>0</v>
       </c>
-      <c r="V9" s="3">
-        <v>0</v>
-      </c>
-      <c r="W9" s="4">
+      <c r="V9" s="4">
+        <v>0</v>
+      </c>
+      <c r="W9" s="3">
         <v>0</v>
       </c>
       <c r="X9" s="4">
         <v>0</v>
       </c>
-      <c r="Y9" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="4">
+      <c r="Y9" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="3">
         <v>0</v>
       </c>
       <c r="AA9" s="4">
         <v>0</v>
       </c>
-      <c r="AB9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC9" s="4">
+      <c r="AB9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="3">
         <v>0</v>
       </c>
       <c r="AD9" s="4">
         <v>0</v>
       </c>
-      <c r="AE9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF9" s="4">
+      <c r="AE9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="3">
         <v>0</v>
       </c>
       <c r="AG9" s="4">
         <v>0</v>
       </c>
-      <c r="AH9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AI9" s="4">
+      <c r="AH9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI9" s="3">
         <v>0</v>
       </c>
       <c r="AJ9" s="4">
         <v>0</v>
       </c>
-      <c r="AK9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AL9" s="4">
+      <c r="AK9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL9" s="3">
         <v>0</v>
       </c>
       <c r="AM9" s="4">
         <v>0</v>
       </c>
-      <c r="AN9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AO9" s="4">
+      <c r="AN9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AO9" s="3">
         <v>0</v>
       </c>
       <c r="AP9" s="4">
         <v>0</v>
       </c>
-      <c r="AQ9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AR9" s="4">
+      <c r="AQ9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR9" s="3">
         <v>0</v>
       </c>
       <c r="AS9" s="4">
         <v>0</v>
       </c>
-      <c r="AT9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AU9" s="4">
+      <c r="AT9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AU9" s="3">
         <v>0</v>
       </c>
       <c r="AV9" s="4">
         <v>0</v>
       </c>
-      <c r="AW9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AX9" s="4">
+      <c r="AW9" s="4">
+        <v>0</v>
+      </c>
+      <c r="AX9" s="3">
         <v>0</v>
       </c>
       <c r="AY9" s="4">
         <v>0</v>
       </c>
-      <c r="AZ9" s="3">
-        <v>0</v>
-      </c>
-      <c r="BA9" s="4">
+      <c r="AZ9" s="4">
+        <v>0</v>
+      </c>
+      <c r="BA9" s="3">
         <v>0</v>
       </c>
       <c r="BB9" s="4">
         <v>0</v>
       </c>
-      <c r="BC9" s="3">
-        <v>0</v>
-      </c>
-      <c r="BD9" s="4">
+      <c r="BC9" s="4">
+        <v>0</v>
+      </c>
+      <c r="BD9" s="3">
         <v>0</v>
       </c>
       <c r="BE9" s="4">
         <v>0</v>
       </c>
-      <c r="BF9" s="3">
-        <v>0</v>
-      </c>
-      <c r="BG9" s="4">
+      <c r="BF9" s="4">
+        <v>0</v>
+      </c>
+      <c r="BG9" s="3">
         <v>0</v>
       </c>
       <c r="BH9" s="4">
         <v>0</v>
       </c>
-      <c r="BI9" s="3">
-        <v>0</v>
-      </c>
-      <c r="BJ9" s="4">
+      <c r="BI9" s="4">
+        <v>0</v>
+      </c>
+      <c r="BJ9" s="3">
         <v>0</v>
       </c>
       <c r="BK9" s="4">
         <v>0</v>
       </c>
-      <c r="BL9" s="3">
-        <v>0</v>
-      </c>
-      <c r="BM9" s="4">
-        <v>0</v>
-      </c>
-      <c r="BN9" s="3">
+      <c r="BL9" s="4">
+        <v>0</v>
+      </c>
+      <c r="BM9" s="3">
+        <v>0</v>
+      </c>
+      <c r="BN9" s="4">
         <v>0</v>
       </c>
       <c r="BO9" s="3">
@@ -1683,10 +1711,13 @@
         <v>0</v>
       </c>
       <c r="BV9" s="3">
+        <v>0</v>
+      </c>
+      <c r="BW9" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:74" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:75" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1694,195 +1725,195 @@
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="3">
+      <c r="E10" s="3">
         <v>10.59262</v>
       </c>
-      <c r="E10" s="4">
+      <c r="F10" s="4">
         <v>1</v>
       </c>
-      <c r="F10" s="4">
-        <v>0</v>
-      </c>
-      <c r="G10" s="3">
+      <c r="G10" s="4">
+        <v>0</v>
+      </c>
+      <c r="H10" s="3">
         <v>1</v>
       </c>
-      <c r="H10" s="4">
-        <v>0</v>
-      </c>
       <c r="I10" s="4">
         <v>0</v>
       </c>
-      <c r="J10" s="3">
-        <v>0</v>
-      </c>
-      <c r="K10" s="4">
+      <c r="J10" s="4">
+        <v>0</v>
+      </c>
+      <c r="K10" s="3">
         <v>0</v>
       </c>
       <c r="L10" s="4">
         <v>0</v>
       </c>
-      <c r="M10" s="3">
-        <v>0</v>
-      </c>
-      <c r="N10" s="4">
+      <c r="M10" s="4">
+        <v>0</v>
+      </c>
+      <c r="N10" s="3">
         <v>0</v>
       </c>
       <c r="O10" s="4">
         <v>0</v>
       </c>
-      <c r="P10" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="4">
+      <c r="P10" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="3">
         <v>0</v>
       </c>
       <c r="R10" s="4">
         <v>0</v>
       </c>
-      <c r="S10" s="3">
-        <v>0</v>
-      </c>
-      <c r="T10" s="4">
+      <c r="S10" s="4">
+        <v>0</v>
+      </c>
+      <c r="T10" s="3">
         <v>0</v>
       </c>
       <c r="U10" s="4">
         <v>0</v>
       </c>
-      <c r="V10" s="3">
-        <v>0</v>
-      </c>
-      <c r="W10" s="4">
+      <c r="V10" s="4">
+        <v>0</v>
+      </c>
+      <c r="W10" s="3">
         <v>0</v>
       </c>
       <c r="X10" s="4">
         <v>0</v>
       </c>
-      <c r="Y10" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="4">
+      <c r="Y10" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="3">
         <v>0</v>
       </c>
       <c r="AA10" s="4">
         <v>0</v>
       </c>
-      <c r="AB10" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC10" s="4">
+      <c r="AB10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="3">
         <v>0</v>
       </c>
       <c r="AD10" s="4">
         <v>0</v>
       </c>
-      <c r="AE10" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF10" s="4">
+      <c r="AE10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="3">
         <v>0</v>
       </c>
       <c r="AG10" s="4">
         <v>0</v>
       </c>
-      <c r="AH10" s="3">
-        <v>0</v>
-      </c>
-      <c r="AI10" s="4">
+      <c r="AH10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI10" s="3">
         <v>0</v>
       </c>
       <c r="AJ10" s="4">
         <v>0</v>
       </c>
-      <c r="AK10" s="3">
-        <v>0</v>
-      </c>
-      <c r="AL10" s="4">
+      <c r="AK10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL10" s="3">
         <v>0</v>
       </c>
       <c r="AM10" s="4">
         <v>0</v>
       </c>
-      <c r="AN10" s="3">
-        <v>0</v>
-      </c>
-      <c r="AO10" s="4">
+      <c r="AN10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AO10" s="3">
         <v>0</v>
       </c>
       <c r="AP10" s="4">
         <v>0</v>
       </c>
-      <c r="AQ10" s="3">
-        <v>0</v>
-      </c>
-      <c r="AR10" s="4">
+      <c r="AQ10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR10" s="3">
         <v>0</v>
       </c>
       <c r="AS10" s="4">
         <v>0</v>
       </c>
-      <c r="AT10" s="3">
-        <v>0</v>
-      </c>
-      <c r="AU10" s="4">
+      <c r="AT10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AU10" s="3">
         <v>0</v>
       </c>
       <c r="AV10" s="4">
         <v>0</v>
       </c>
-      <c r="AW10" s="3">
-        <v>0</v>
-      </c>
-      <c r="AX10" s="4">
+      <c r="AW10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AX10" s="3">
         <v>0</v>
       </c>
       <c r="AY10" s="4">
         <v>0</v>
       </c>
-      <c r="AZ10" s="3">
-        <v>0</v>
-      </c>
-      <c r="BA10" s="4">
+      <c r="AZ10" s="4">
+        <v>0</v>
+      </c>
+      <c r="BA10" s="3">
         <v>0</v>
       </c>
       <c r="BB10" s="4">
         <v>0</v>
       </c>
-      <c r="BC10" s="3">
-        <v>0</v>
-      </c>
-      <c r="BD10" s="4">
+      <c r="BC10" s="4">
+        <v>0</v>
+      </c>
+      <c r="BD10" s="3">
         <v>0</v>
       </c>
       <c r="BE10" s="4">
         <v>0</v>
       </c>
-      <c r="BF10" s="3">
-        <v>0</v>
-      </c>
-      <c r="BG10" s="4">
+      <c r="BF10" s="4">
+        <v>0</v>
+      </c>
+      <c r="BG10" s="3">
         <v>0</v>
       </c>
       <c r="BH10" s="4">
         <v>0</v>
       </c>
-      <c r="BI10" s="3">
-        <v>0</v>
-      </c>
-      <c r="BJ10" s="4">
+      <c r="BI10" s="4">
+        <v>0</v>
+      </c>
+      <c r="BJ10" s="3">
         <v>0</v>
       </c>
       <c r="BK10" s="4">
         <v>0</v>
       </c>
-      <c r="BL10" s="3">
-        <v>0</v>
-      </c>
-      <c r="BM10" s="4">
-        <v>0</v>
-      </c>
-      <c r="BN10" s="3">
+      <c r="BL10" s="4">
+        <v>0</v>
+      </c>
+      <c r="BM10" s="3">
+        <v>0</v>
+      </c>
+      <c r="BN10" s="4">
         <v>0</v>
       </c>
       <c r="BO10" s="3">
@@ -1907,10 +1938,13 @@
         <v>0</v>
       </c>
       <c r="BV10" s="3">
+        <v>0</v>
+      </c>
+      <c r="BW10" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:74" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:75" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -1918,195 +1952,195 @@
         <v>11</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="3">
+      <c r="E11" s="3">
         <v>12.21255</v>
       </c>
-      <c r="E11" s="4">
+      <c r="F11" s="4">
         <v>1</v>
       </c>
-      <c r="F11" s="4">
-        <v>0</v>
-      </c>
-      <c r="G11" s="3">
+      <c r="G11" s="4">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3">
         <v>1</v>
       </c>
-      <c r="H11" s="4">
-        <v>0</v>
-      </c>
       <c r="I11" s="4">
         <v>0</v>
       </c>
-      <c r="J11" s="3">
-        <v>0</v>
-      </c>
-      <c r="K11" s="4">
+      <c r="J11" s="4">
+        <v>0</v>
+      </c>
+      <c r="K11" s="3">
         <v>0</v>
       </c>
       <c r="L11" s="4">
         <v>0</v>
       </c>
-      <c r="M11" s="3">
-        <v>0</v>
-      </c>
-      <c r="N11" s="4">
+      <c r="M11" s="4">
+        <v>0</v>
+      </c>
+      <c r="N11" s="3">
         <v>0</v>
       </c>
       <c r="O11" s="4">
         <v>0</v>
       </c>
-      <c r="P11" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="4">
+      <c r="P11" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="3">
         <v>0</v>
       </c>
       <c r="R11" s="4">
         <v>0</v>
       </c>
-      <c r="S11" s="3">
-        <v>0</v>
-      </c>
-      <c r="T11" s="4">
+      <c r="S11" s="4">
+        <v>0</v>
+      </c>
+      <c r="T11" s="3">
         <v>0</v>
       </c>
       <c r="U11" s="4">
         <v>0</v>
       </c>
-      <c r="V11" s="3">
-        <v>0</v>
-      </c>
-      <c r="W11" s="4">
+      <c r="V11" s="4">
+        <v>0</v>
+      </c>
+      <c r="W11" s="3">
         <v>0</v>
       </c>
       <c r="X11" s="4">
         <v>0</v>
       </c>
-      <c r="Y11" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="4">
+      <c r="Y11" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="3">
         <v>0</v>
       </c>
       <c r="AA11" s="4">
         <v>0</v>
       </c>
-      <c r="AB11" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC11" s="4">
+      <c r="AB11" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="3">
         <v>0</v>
       </c>
       <c r="AD11" s="4">
         <v>0</v>
       </c>
-      <c r="AE11" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF11" s="4">
+      <c r="AE11" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF11" s="3">
         <v>0</v>
       </c>
       <c r="AG11" s="4">
         <v>0</v>
       </c>
-      <c r="AH11" s="3">
-        <v>0</v>
-      </c>
-      <c r="AI11" s="4">
+      <c r="AH11" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI11" s="3">
         <v>0</v>
       </c>
       <c r="AJ11" s="4">
         <v>0</v>
       </c>
-      <c r="AK11" s="3">
-        <v>0</v>
-      </c>
-      <c r="AL11" s="4">
+      <c r="AK11" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL11" s="3">
         <v>0</v>
       </c>
       <c r="AM11" s="4">
         <v>0</v>
       </c>
-      <c r="AN11" s="3">
-        <v>0</v>
-      </c>
-      <c r="AO11" s="4">
+      <c r="AN11" s="4">
+        <v>0</v>
+      </c>
+      <c r="AO11" s="3">
         <v>0</v>
       </c>
       <c r="AP11" s="4">
         <v>0</v>
       </c>
-      <c r="AQ11" s="3">
-        <v>0</v>
-      </c>
-      <c r="AR11" s="4">
+      <c r="AQ11" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR11" s="3">
         <v>0</v>
       </c>
       <c r="AS11" s="4">
         <v>0</v>
       </c>
-      <c r="AT11" s="3">
-        <v>0</v>
-      </c>
-      <c r="AU11" s="4">
+      <c r="AT11" s="4">
+        <v>0</v>
+      </c>
+      <c r="AU11" s="3">
         <v>0</v>
       </c>
       <c r="AV11" s="4">
         <v>0</v>
       </c>
-      <c r="AW11" s="3">
-        <v>0</v>
-      </c>
-      <c r="AX11" s="4">
+      <c r="AW11" s="4">
+        <v>0</v>
+      </c>
+      <c r="AX11" s="3">
         <v>0</v>
       </c>
       <c r="AY11" s="4">
         <v>0</v>
       </c>
-      <c r="AZ11" s="3">
-        <v>0</v>
-      </c>
-      <c r="BA11" s="4">
+      <c r="AZ11" s="4">
+        <v>0</v>
+      </c>
+      <c r="BA11" s="3">
         <v>0</v>
       </c>
       <c r="BB11" s="4">
         <v>0</v>
       </c>
-      <c r="BC11" s="3">
-        <v>0</v>
-      </c>
-      <c r="BD11" s="4">
+      <c r="BC11" s="4">
+        <v>0</v>
+      </c>
+      <c r="BD11" s="3">
         <v>0</v>
       </c>
       <c r="BE11" s="4">
         <v>0</v>
       </c>
-      <c r="BF11" s="3">
-        <v>0</v>
-      </c>
-      <c r="BG11" s="4">
+      <c r="BF11" s="4">
+        <v>0</v>
+      </c>
+      <c r="BG11" s="3">
         <v>0</v>
       </c>
       <c r="BH11" s="4">
         <v>0</v>
       </c>
-      <c r="BI11" s="3">
-        <v>0</v>
-      </c>
-      <c r="BJ11" s="4">
+      <c r="BI11" s="4">
+        <v>0</v>
+      </c>
+      <c r="BJ11" s="3">
         <v>0</v>
       </c>
       <c r="BK11" s="4">
         <v>0</v>
       </c>
-      <c r="BL11" s="3">
-        <v>0</v>
-      </c>
-      <c r="BM11" s="4">
-        <v>0</v>
-      </c>
-      <c r="BN11" s="3">
+      <c r="BL11" s="4">
+        <v>0</v>
+      </c>
+      <c r="BM11" s="3">
+        <v>0</v>
+      </c>
+      <c r="BN11" s="4">
         <v>0</v>
       </c>
       <c r="BO11" s="3">
@@ -2131,6 +2165,9 @@
         <v>0</v>
       </c>
       <c r="BV11" s="3">
+        <v>0</v>
+      </c>
+      <c r="BW11" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>